<commit_message>
adding validation to sdtables cli
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cunningr/git-projects/sdtables/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18E9C8D-76FF-7E4A-9DF2-9A35A7262873}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA6C1FF-4834-164F-8D2F-9DC84661F6B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{4F14C34B-327E-6C49-AD9F-2C718CE96282}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEB751A-DBDC-1F4B-BDB3-A0AC83845032}" name="super.heros" displayName="super.heros" ref="B3:F7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEB751A-DBDC-1F4B-BDB3-A0AC83845032}" name="super.heroes" displayName="super.heroes" ref="B3:F7" totalsRowShown="0">
   <autoFilter ref="B3:F7" xr:uid="{2BA2BB69-2757-DE49-A466-AC55595EC469}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{05DD279A-D5AB-3D49-B1D0-F205088C2B27}" name="Name"/>
@@ -511,7 +511,7 @@
   <dimension ref="B3:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>